<commit_message>
Task 1 & Task 2 completion
</commit_message>
<xml_diff>
--- a/Automate.io/Configuration/Config.xlsx
+++ b/Automate.io/Configuration/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="5985" tabRatio="787" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="5985" tabRatio="787" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="2" r:id="rId1"/>
@@ -139,12 +139,6 @@
     <t>PerformTask2</t>
   </si>
   <si>
-    <t>{
-"username":"raviauto09@gmail.com",
-"password":"2589243m"
-}</t>
-  </si>
-  <si>
     <t>AutomateIOSuite</t>
   </si>
   <si>
@@ -155,6 +149,12 @@
 "newMailFolderName":"INBOX",
 "toName":"Ravindra Kumar",
 "toAddress":"rkumar124795@gmail.com"
+}</t>
+  </si>
+  <si>
+    <t>{
+"username":"rkumar124795@gmail.com",
+"password":"2589243m"
 }</t>
   </si>
 </sst>
@@ -330,6 +330,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -341,15 +350,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -746,7 +746,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>31</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>35</v>
@@ -905,10 +905,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -936,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,7 +964,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>35</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>35</v>
@@ -991,10 +991,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1022,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,26 +1048,26 @@
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>39</v>
+      <c r="C2" s="19" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="24"/>
+      <c r="C11" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
@@ -1113,9 +1113,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1149,7 +1149,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>12</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>13</v>
@@ -1165,15 +1165,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>